<commit_message>
Working - loading and parsing
</commit_message>
<xml_diff>
--- a/data/raw/U16432685_202501_202501_parsed.xlsx
+++ b/data/raw/U16432685_202501_202501_parsed.xlsx
@@ -19,6 +19,7 @@
     <sheet name="Broker Interest Received" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Bond Interest Paid" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="Bond Interest Received" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Financial Instrument Informatio" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3672,6 +3673,797 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Asset Category</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Conid</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Security ID</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Underlying</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Listing Exch</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Multiplier</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Code</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Stocks</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AEEM</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>AMUNDI MSCI EMERG MARK</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>314449552</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>LU1681045370</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>AEEM</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>SBF</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>ETF</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Stocks</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>AJG</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ARTHUR J GALLAGHER &amp; CO</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>4325</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>US3635761097</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>AJG</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>COMMON</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Stocks</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BXMT</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>BLACKSTONE MORTGAGE TRU-CL A</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>127149807</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>US09257W1009</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>BXMT</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>REIT</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Stocks</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CSPX</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ISHARES CORE S&amp;P 500</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>75776072</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>IE00B5BMR087</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>SXR8</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>IBIS2</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>ETF</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Stocks</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CSX</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CSX CORP</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>6150</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>US1264081035</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>CSX</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>COMMON</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Stocks</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>EMD</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>WESTERN ASSET EMRG MRKT DBT</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>41073515</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>US95766A1016</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>EMD</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>CLOSED-END FUND</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Stocks</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>GLD</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SPDR GOLD SHARES</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>51529211</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>US78463V1070</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>GLD</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>ARCA</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>ETF</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Stocks</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>JPC</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NUVEEN PREFERED &amp; INCOME OPP</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>17635192</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>US67073B1061</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>JPC</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>CLOSED-END FUND</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Stocks</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>LRCX</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>LAM RESEARCH CORP</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>732440574</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>US5128073062</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>LRCX</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>COMMON</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Stocks</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ALTRIA GROUP INC</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>9769</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>US02209S1033</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>COMMON</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Stocks</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>QRTEP</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>QURATE RETAIL INC</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>442948738</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>US74915M3088</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>QRTEP</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>PUBLIC</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Stocks</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>RGLD</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ROYAL GOLD INC</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>4817403</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>US7802871084</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>RGLD</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>COMMON</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Stocks</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>TLT</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ISHARES 20+ YEAR TREASURY BD</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>15547841</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>US4642874329</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>TLT</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>ETF</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Stocks</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>VISA INC-CLASS A SHARES</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>49462172</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>US92826C8394</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>COMMON</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Stocks</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>XLB</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>MATERIALS SELECT SECTOR SPDR</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>4215200</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>US81369Y1001</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>XLB</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>ARCA</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>ETF</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -5342,7 +6134,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5371,11 +6163,6 @@
           <t>Amount</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Code</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -5398,7 +6185,6 @@
           <t>230</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -5421,7 +6207,6 @@
           <t>2244</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -5444,7 +6229,6 @@
           <t>2820</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -5467,7 +6251,6 @@
           <t>135</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -5482,7 +6265,6 @@
           <t>5429</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -5497,129 +6279,6 @@
           <t>5284.95026</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2025-01-08</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>LRCX(US5128073062) Cash Dividend USD 0.23 per Share (Ordinary Dividend)</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>230</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2025-01-10</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>MO(US02209S1033) Cash Dividend USD 1.02 per Share (Ordinary Dividend)</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2244</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2025-01-15</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>BXMT(US09257W1009) Cash Dividend USD 0.47 per Share (Ordinary Dividend)</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2820</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2025-01-17</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>RGLD(US7802871084) Cash Dividend USD 0.45 per Share (Ordinary Dividend)</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>135</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>5429</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Total in EUR</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>5284.95026</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
P&L table fully functional. No FX conversion for Trading Profit.
</commit_message>
<xml_diff>
--- a/data/raw/U16432685_202501_202501_parsed.xlsx
+++ b/data/raw/U16432685_202501_202501_parsed.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Realized &amp; Unrealized Performance Summary</t>
+          <t>Trading Profit</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -453,80 +453,40 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Dividends</t>
+          <t>Net Dividend Income</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5284.95026</v>
+        <v>4773.629295799999</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Withholding Tax</t>
+          <t>Net Interest Profit</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-511.3209642</v>
+        <v>13869.468039</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Other Fees</t>
+          <t>OpEx</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-120.98</v>
+        <v>-147.444</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Sales Tax Details</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-26.464</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Broker Interest Received</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>152.6900162</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Bond Interest Paid</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>-1424.7173144</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Bond Interest Received</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>15141.4953372</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
         <v>26526.53446901</v>
       </c>
     </row>

</xml_diff>